<commit_message>
changing individual course page term to list all terms
</commit_message>
<xml_diff>
--- a/markdown_generator/teaching.xlsx
+++ b/markdown_generator/teaching.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="164">
   <si>
     <t>term</t>
   </si>
@@ -432,9 +432,6 @@
   </si>
   <si>
     <t>This course introduces students to the basics of propositional and predicate logic in symbolizing natural language and determining validity, and introduces such topics as the logic of set theory, functions, relations, and transfinite sets. Emphasis is placed upon strategies involved in constructing proofs.</t>
-  </si>
-  <si>
-    <t>MATH/CPSC 212</t>
   </si>
   <si>
     <t>This course investigates applications of modeling techniques used in a variety of disciplines, including the natural sciences, mathematics, computer science and business. The nature and use of calculus (both differential and integral) is a primary focus of the course.</t>
@@ -513,13 +510,7 @@
     <t>This course covers: operations with numeric and algebraic expressions, polynomials, rational expressions and equations, roots, radicals and complex numbers, linear equations/functions and graphing, systems of linear equations and inequalities, quadratic functions, and exponential and logarithmic functions.</t>
   </si>
   <si>
-    <t>MATH/CPSC: 140</t>
-  </si>
-  <si>
     <t>This course is an introduction to set theory, logic, integers, combinatorics, and functions for today's computer scientists.</t>
-  </si>
-  <si>
-    <t>MATH/CPSC: 340</t>
   </si>
   <si>
     <t>Topics included are propositional logic, set theory, graph theory and combinatorial analysis, and Boolean algebra. Applications and theory are discussed.</t>
@@ -2340,7 +2331,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>140</v>
+        <v>71</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>72</v>
@@ -2352,7 +2343,7 @@
         <v>46</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9">
@@ -2369,7 +2360,7 @@
         <v>46</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10">
@@ -2386,7 +2377,7 @@
         <v>46</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11">
@@ -2403,7 +2394,7 @@
         <v>46</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12">
@@ -2420,7 +2411,7 @@
         <v>90</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13">
@@ -2437,7 +2428,7 @@
         <v>90</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14">
@@ -2454,7 +2445,7 @@
         <v>17</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15">
@@ -2471,7 +2462,7 @@
         <v>90</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16">
@@ -2488,7 +2479,7 @@
         <v>90</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17">
@@ -2505,7 +2496,7 @@
         <v>90</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18">
@@ -2522,7 +2513,7 @@
         <v>90</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19">
@@ -2539,7 +2530,7 @@
         <v>90</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20">
@@ -2556,7 +2547,7 @@
         <v>90</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="21">
@@ -2573,7 +2564,7 @@
         <v>90</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22">
@@ -2590,7 +2581,7 @@
         <v>90</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="23">
@@ -2607,7 +2598,7 @@
         <v>17</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="24">
@@ -2624,7 +2615,7 @@
         <v>33</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25">
@@ -2641,7 +2632,7 @@
         <v>90</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="26">
@@ -2658,7 +2649,7 @@
         <v>17</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27">
@@ -2675,7 +2666,7 @@
         <v>33</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="28">
@@ -2692,7 +2683,7 @@
         <v>17</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="29">
@@ -2709,12 +2700,12 @@
         <v>46</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>162</v>
+        <v>16</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>47</v>
@@ -2726,12 +2717,12 @@
         <v>46</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>164</v>
+        <v>49</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>50</v>
@@ -2743,7 +2734,7 @@
         <v>46</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="32">
@@ -2760,7 +2751,7 @@
         <v>46</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add winter 2022, spring 2022 to teaching
</commit_message>
<xml_diff>
--- a/markdown_generator/teaching.xlsx
+++ b/markdown_generator/teaching.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="170">
   <si>
     <t>term</t>
   </si>
@@ -411,6 +411,21 @@
   </si>
   <si>
     <t>Fall 2021</t>
+  </si>
+  <si>
+    <t>Winter 2022</t>
+  </si>
+  <si>
+    <t>Spring 2022</t>
+  </si>
+  <si>
+    <t>CDS 1020</t>
+  </si>
+  <si>
+    <t>Introduction to Computational Data Science</t>
+  </si>
+  <si>
+    <t>class-27</t>
   </si>
   <si>
     <t>description</t>
@@ -517,18 +532,23 @@
   </si>
   <si>
     <t>This course is a college preparatory course designed for students who need to learn or revisit concepts typically taught in a high school Algebra I course. This course covers the fundamentals of arithmetic skills necessary in daily life and builds a foundation of algebraic understanding. Topics included are: operations with real numbers, percent, ratio, proportion, expressions, linear equations, polynomials, and radicals.</t>
+  </si>
+  <si>
+    <t>Goals: To continue the study of computational techniques using Python, with an emphasis on applications in data science and analytics.
+Content: This is a continuation of CDS 1010, applying algorithmic thinking to applications in data analysis. Topics include data mining, data visualization, web-scraping.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font/>
   </fonts>
   <fills count="3">
     <fill>
@@ -550,11 +570,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -2191,6 +2214,86 @@
         <v>91</v>
       </c>
     </row>
+    <row r="81">
+      <c r="A81" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -2224,7 +2327,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2">
@@ -2240,8 +2343,8 @@
       <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>134</v>
+      <c r="E2" s="3" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="3">
@@ -2258,7 +2361,7 @@
         <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4">
@@ -2275,7 +2378,7 @@
         <v>46</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5">
@@ -2292,7 +2395,7 @@
         <v>46</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6">
@@ -2309,7 +2412,7 @@
         <v>46</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7">
@@ -2326,7 +2429,7 @@
         <v>46</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8">
@@ -2343,7 +2446,7 @@
         <v>46</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9">
@@ -2360,7 +2463,7 @@
         <v>46</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10">
@@ -2377,7 +2480,7 @@
         <v>46</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11">
@@ -2394,7 +2497,7 @@
         <v>46</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
     <row r="12">
@@ -2411,7 +2514,7 @@
         <v>90</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13">
@@ -2428,7 +2531,7 @@
         <v>90</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14">
@@ -2445,7 +2548,7 @@
         <v>17</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15">
@@ -2462,7 +2565,7 @@
         <v>90</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16">
@@ -2479,7 +2582,7 @@
         <v>90</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17">
@@ -2496,7 +2599,7 @@
         <v>90</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18">
@@ -2512,8 +2615,8 @@
       <c r="D18" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>149</v>
+      <c r="E18" s="3" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="19">
@@ -2529,8 +2632,8 @@
       <c r="D19" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>150</v>
+      <c r="E19" s="3" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="20">
@@ -2547,7 +2650,7 @@
         <v>90</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
     </row>
     <row r="21">
@@ -2564,7 +2667,7 @@
         <v>90</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
     </row>
     <row r="22">
@@ -2581,7 +2684,7 @@
         <v>90</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23">
@@ -2598,7 +2701,7 @@
         <v>17</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24">
@@ -2614,8 +2717,8 @@
       <c r="D24" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>155</v>
+      <c r="E24" s="3" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="25">
@@ -2632,7 +2735,7 @@
         <v>90</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
     </row>
     <row r="26">
@@ -2649,7 +2752,7 @@
         <v>17</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="27">
@@ -2665,8 +2768,8 @@
       <c r="D27" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>158</v>
+      <c r="E27" s="3" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="28">
@@ -2683,7 +2786,7 @@
         <v>17</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
     </row>
     <row r="29">
@@ -2700,7 +2803,7 @@
         <v>46</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
     </row>
     <row r="30">
@@ -2717,7 +2820,7 @@
         <v>46</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
     </row>
     <row r="31">
@@ -2734,7 +2837,7 @@
         <v>46</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
     </row>
     <row r="32">
@@ -2751,7 +2854,24 @@
         <v>46</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>163</v>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>